<commit_message>
Sprint-1 : Week-1: Tests are included.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeapThoughtProjectWS\FluidTX_Trunk\src\com\proj\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-IssuedForInformation.xlsx</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_New_IssuedForReview</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_New_RequestForInformation</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_New_IssuedForApproval</t>
+  </si>
+  <si>
+    <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-IssuedForReview.xlsx</t>
+  </si>
+  <si>
+    <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-RequestForInformation.xlsx</t>
+  </si>
+  <si>
+    <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-IssuedForApproval.xlsx</t>
   </si>
 </sst>
 </file>
@@ -529,11 +547,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -597,9 +613,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -611,11 +651,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -701,6 +739,39 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -709,10 +780,13 @@
     <hyperlink ref="B4" r:id="rId4"/>
     <hyperlink ref="B5" r:id="rId5"/>
     <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Included FLD_DocumentRegistry_New_Transmittals test details
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-IssuedForApproval.xlsx</t>
+  </si>
+  <si>
+    <t>FLD_DocumentRegistry_New_Transmittals</t>
+  </si>
+  <si>
+    <t>\\src\\com\\proj\\suiteDOCS\\testdata\\DocumentRegistryTestData-Newtransmittal.xlsx</t>
   </si>
 </sst>
 </file>
@@ -547,9 +553,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -637,9 +645,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B11">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -651,9 +667,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -772,6 +790,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -783,10 +812,11 @@
     <hyperlink ref="B8" r:id="rId7"/>
     <hyperlink ref="B9" r:id="rId8"/>
     <hyperlink ref="B10" r:id="rId9"/>
+    <hyperlink ref="B11" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Included Action Required tests
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>\\src\\com\\proj\\suiteDOCS\\testdata\\DocumentRegistryTestData-Newtransmittal.xlsx</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_ActionRequired_New_RequestForInformation</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_ActionRequired_New_IssuedForReview</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_ActionRequired_New_IssuedForApproval</t>
   </si>
 </sst>
 </file>
@@ -553,11 +562,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -653,9 +660,33 @@
         <v>2</v>
       </c>
     </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B14">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -667,11 +698,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -798,6 +827,39 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -813,10 +875,13 @@
     <hyperlink ref="B9" r:id="rId8"/>
     <hyperlink ref="B10" r:id="rId9"/>
     <hyperlink ref="B11" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B12" r:id="rId12"/>
+    <hyperlink ref="B14" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId11"/>
+  <legacyDrawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Included FLD_Transmittals_LeftNavigationBar 2. Changed the data sheet name for all action required tests.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-IssuedForApproval-CancelAndClose.xlsx</t>
+  </si>
+  <si>
+    <t>Transmittals_New_ActionRequired</t>
+  </si>
+  <si>
+    <t>FLD_Transmittals_LeftNavigationBar</t>
+  </si>
+  <si>
+    <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\Transmittals-Fluid-Navigation.xlsx</t>
+  </si>
+  <si>
+    <t>Fluid_Navigation</t>
   </si>
 </sst>
 </file>
@@ -583,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -731,9 +743,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B18">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -745,10 +765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -887,7 +907,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -898,7 +918,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -909,7 +929,7 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -943,6 +963,17 @@
       </c>
       <c r="C17" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -963,10 +994,11 @@
     <hyperlink ref="B15" r:id="rId14"/>
     <hyperlink ref="B16" r:id="rId15"/>
     <hyperlink ref="B17" r:id="rId16"/>
+    <hyperlink ref="B18" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId17"/>
+  <legacyDrawing r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test data document name changed
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14865" windowHeight="2820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14865" windowHeight="2820"/>
   </bookViews>
   <sheets>
     <sheet name="DataFetchFlag" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -192,7 +192,10 @@
     <t>FLD_CreateNewDocument</t>
   </si>
   <si>
-    <t xml:space="preserve">\\src\\com\\proj\\suiteDOCS\\testdata\\FLD_CreateNewDocument.xlsx </t>
+    <t xml:space="preserve">\\src\\com\\proj\\suiteDOCS\\testdata\\Documents_CreateNewDocument.xlsx </t>
+  </si>
+  <si>
+    <t>Documents_CreateNewDocument</t>
   </si>
 </sst>
 </file>
@@ -615,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -787,7 +790,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>2</v>
@@ -809,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1048,7 +1051,7 @@
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected the test name to FLD_CreateNewDocument
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/config/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_May\Fulcrum_FluidTX_Trunk\src\com\proj\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -790,7 +790,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>2</v>
@@ -812,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>